<commit_message>
Import and analyze tandem measurement data
</commit_message>
<xml_diff>
--- a/inputs/dma_params_2d.xlsx
+++ b/inputs/dma_params_2d.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hmdni\OneDrive\Documents\GitHub\odias\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1582F61A-D173-4086-9E03-2A2312A83BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AEA1DB-CB24-4603-A60F-7140874D9CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{BF76CB6B-6024-45E4-967E-95DB60FBF193}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BF76CB6B-6024-45E4-967E-95DB60FBF193}"/>
   </bookViews>
   <sheets>
-    <sheet name="26JUL24" sheetId="7" r:id="rId1"/>
-    <sheet name="30JUL24" sheetId="8" r:id="rId2"/>
+    <sheet name="21AUG24" sheetId="9" r:id="rId1"/>
+    <sheet name="20AUG24_1" sheetId="10" r:id="rId2"/>
+    <sheet name="30JUL24" sheetId="8" r:id="rId3"/>
+    <sheet name="26JUL24" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="62">
   <si>
     <t>f_add</t>
   </si>
@@ -142,6 +144,87 @@
   </si>
   <si>
     <t>2024-07-30_203242_SMPS</t>
+  </si>
+  <si>
+    <t>D:\Hamed\CND\PhD\Experiments\PFA-RH122\PFA results\SMPS\Post-processed\ET+NIT\21AUG24\Dens</t>
+  </si>
+  <si>
+    <t>2024-08-21_204424_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-21_210317_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-21_211711_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-21_213243_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-21_221937_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-21_223237_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-21_224530_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-21_230056_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-21_231418_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-21_232708_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-22_003114_SMPS</t>
+  </si>
+  <si>
+    <t>6:8</t>
+  </si>
+  <si>
+    <t>9:11</t>
+  </si>
+  <si>
+    <t>12:14</t>
+  </si>
+  <si>
+    <t>7:9</t>
+  </si>
+  <si>
+    <t>4:10</t>
+  </si>
+  <si>
+    <t>D:\Hamed\CND\PhD\Experiments\PFA-RH122\PFA results\SMPS\Post-processed\ET+NIT\20AUG24_1\Dens</t>
+  </si>
+  <si>
+    <t>2024-08-20_133417_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-20_141312_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-20_145039_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-20_150406_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-20_151851_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-20_153447_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-20_154754_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-20_164029_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-20_171355_SMPS</t>
   </si>
 </sst>
 </file>
@@ -531,6 +614,1028 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5412BFC8-26D3-4882-BCC3-6D9CC7342A11}">
+  <dimension ref="A1:H51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="5">
+        <v>43.3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3.92</v>
+      </c>
+      <c r="E2" s="4">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="5">
+        <v>50.8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4.62</v>
+      </c>
+      <c r="E3" s="4">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="5">
+        <v>59.5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5.41</v>
+      </c>
+      <c r="E4" s="4">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="5">
+        <v>69.7</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6.34</v>
+      </c>
+      <c r="E5" s="4">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="5">
+        <v>81.7</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7.42</v>
+      </c>
+      <c r="E6" s="4">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="5">
+        <v>95.8</v>
+      </c>
+      <c r="D7" s="2">
+        <v>8.68</v>
+      </c>
+      <c r="E7" s="4">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="5">
+        <v>112.3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>10.1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5">
+        <v>131.6</v>
+      </c>
+      <c r="D9" s="2">
+        <v>11.28</v>
+      </c>
+      <c r="E9" s="4">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="5">
+        <v>154.30000000000001</v>
+      </c>
+      <c r="D10" s="2">
+        <v>12.54</v>
+      </c>
+      <c r="E10" s="4">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="5">
+        <v>180.8</v>
+      </c>
+      <c r="D11" s="2">
+        <v>13.87</v>
+      </c>
+      <c r="E11" s="4">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="5">
+        <v>211.9</v>
+      </c>
+      <c r="D12" s="2">
+        <v>15</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="5">
+        <v>248.4</v>
+      </c>
+      <c r="D13" s="2">
+        <v>15</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="5">
+        <v>291.2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>15</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="C28" s="5"/>
+      <c r="E28" s="4"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+    </row>
+    <row r="48" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="4"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B20DD3B9-5A25-49EE-9856-FE4C94379F05}">
+  <dimension ref="A1:H48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="5">
+        <v>29.130528992918819</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2.63</v>
+      </c>
+      <c r="E2" s="4">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="5">
+        <v>34.135335939708469</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3.09</v>
+      </c>
+      <c r="E3" s="4">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="5">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.63</v>
+      </c>
+      <c r="E4" s="4">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="5">
+        <v>46.9</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4.26</v>
+      </c>
+      <c r="E5" s="4">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="5">
+        <v>55</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="5">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5.83</v>
+      </c>
+      <c r="E7" s="4">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="5">
+        <v>75.5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>6.85</v>
+      </c>
+      <c r="E8" s="4">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="5">
+        <v>88.5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>8.02</v>
+      </c>
+      <c r="E9" s="4">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="5">
+        <v>103.7</v>
+      </c>
+      <c r="D10" s="2">
+        <v>9.36</v>
+      </c>
+      <c r="E10" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="5">
+        <v>121.6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>10.67</v>
+      </c>
+      <c r="E11" s="4">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="5">
+        <v>142.5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>11.89</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="5">
+        <v>167</v>
+      </c>
+      <c r="D13" s="2">
+        <v>13.17</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="5">
+        <v>195.8</v>
+      </c>
+      <c r="D14" s="2">
+        <v>14.55</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="5">
+        <v>229.4</v>
+      </c>
+      <c r="D15" s="2">
+        <v>15</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="C28" s="5"/>
+      <c r="E28" s="4"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+    </row>
+    <row r="48" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="4"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF801D2-98ED-43A7-9E5A-7B2671AE3009}">
+  <dimension ref="A1:H51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5">
+        <v>43.3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3.93</v>
+      </c>
+      <c r="E2" s="4">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="5">
+        <v>50.8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4.63</v>
+      </c>
+      <c r="E3" s="4">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5">
+        <v>59.5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5.42</v>
+      </c>
+      <c r="E4" s="4">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5">
+        <v>69.7</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6.31</v>
+      </c>
+      <c r="E5" s="4">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5">
+        <v>81.7</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7.39</v>
+      </c>
+      <c r="E6" s="4">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="5">
+        <v>95.8</v>
+      </c>
+      <c r="D7" s="2">
+        <v>8.66</v>
+      </c>
+      <c r="E7" s="4">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="5">
+        <v>112.3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>10.07</v>
+      </c>
+      <c r="E8" s="4">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="5">
+        <v>131.6</v>
+      </c>
+      <c r="D9" s="2">
+        <v>11.27</v>
+      </c>
+      <c r="E9" s="4">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5">
+        <v>154.30000000000001</v>
+      </c>
+      <c r="D10" s="2">
+        <v>12.53</v>
+      </c>
+      <c r="E10" s="4">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="5">
+        <v>180.8</v>
+      </c>
+      <c r="D11" s="2">
+        <v>13.87</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="5">
+        <v>211.9</v>
+      </c>
+      <c r="D12" s="2">
+        <v>15</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="5">
+        <v>248.4</v>
+      </c>
+      <c r="D13" s="2">
+        <v>15</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="5">
+        <v>291.2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>15</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="C28" s="5"/>
+      <c r="E28" s="4"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+    </row>
+    <row r="48" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="4"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E154B3E6-2BDE-4817-B65C-F71F8F992F62}">
   <dimension ref="A1:H48"/>
   <sheetViews>
@@ -840,339 +1945,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF801D2-98ED-43A7-9E5A-7B2671AE3009}">
-  <dimension ref="A1:H51"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="5">
-        <v>43.3</v>
-      </c>
-      <c r="D2" s="2">
-        <v>3.93</v>
-      </c>
-      <c r="E2" s="4">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="5">
-        <v>50.8</v>
-      </c>
-      <c r="D3" s="2">
-        <v>4.63</v>
-      </c>
-      <c r="E3" s="4">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3">
-        <v>8</v>
-      </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="5">
-        <v>59.5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>5.42</v>
-      </c>
-      <c r="E4" s="4">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>8</v>
-      </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="5">
-        <v>69.7</v>
-      </c>
-      <c r="D5" s="2">
-        <v>6.31</v>
-      </c>
-      <c r="E5" s="4">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="5">
-        <v>81.7</v>
-      </c>
-      <c r="D6" s="2">
-        <v>7.39</v>
-      </c>
-      <c r="E6" s="4">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="5">
-        <v>95.8</v>
-      </c>
-      <c r="D7" s="2">
-        <v>8.66</v>
-      </c>
-      <c r="E7" s="4">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="5">
-        <v>112.3</v>
-      </c>
-      <c r="D8" s="2">
-        <v>10.07</v>
-      </c>
-      <c r="E8" s="4">
-        <v>4</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="5">
-        <v>131.6</v>
-      </c>
-      <c r="D9" s="2">
-        <v>11.27</v>
-      </c>
-      <c r="E9" s="4">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="5">
-        <v>154.30000000000001</v>
-      </c>
-      <c r="D10" s="2">
-        <v>12.53</v>
-      </c>
-      <c r="E10" s="4">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="5">
-        <v>180.8</v>
-      </c>
-      <c r="D11" s="2">
-        <v>13.87</v>
-      </c>
-      <c r="E11" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="F11" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="5">
-        <v>211.9</v>
-      </c>
-      <c r="D12" s="2">
-        <v>15</v>
-      </c>
-      <c r="E12" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="5">
-        <v>248.4</v>
-      </c>
-      <c r="D13" s="2">
-        <v>15</v>
-      </c>
-      <c r="E13" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="5">
-        <v>291.2</v>
-      </c>
-      <c r="D14" s="2">
-        <v>15</v>
-      </c>
-      <c r="E14" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="C28" s="5"/>
-      <c r="E28" s="4"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-    </row>
-    <row r="48" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="4"/>
-      <c r="F48"/>
-      <c r="G48"/>
-      <c r="H48"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>